<commit_message>
post career fair, keen orders, and subsys layout
</commit_message>
<xml_diff>
--- a/IDEAlab/Copy of TPS_Kern_Purchase_Prefomatted.xlsx
+++ b/IDEAlab/Copy of TPS_Kern_Purchase_Prefomatted.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="75">
   <si>
     <t>DATE</t>
   </si>
@@ -270,6 +270,21 @@
   </si>
   <si>
     <t>DESCRIPTION include hyperlink when possible</t>
+  </si>
+  <si>
+    <t>Pololu</t>
+  </si>
+  <si>
+    <t>https://www.pololu.com/product/3076</t>
+  </si>
+  <si>
+    <t>150:1 Micro Metal Gearmotor HPCB 6V with Extended Motor Shaft</t>
+  </si>
+  <si>
+    <t>Pololu Micro Metal Gearmotor Bracket Pair - Black</t>
+  </si>
+  <si>
+    <t>https://www.pololu.com/product/989</t>
   </si>
 </sst>
 </file>
@@ -540,7 +555,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -813,13 +828,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -1080,8 +1121,65 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1098,66 +1196,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="167" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1178,6 +1216,27 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -1746,8 +1805,8 @@
   </sheetPr>
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1764,14 +1823,14 @@
   <sheetData>
     <row r="1" spans="1:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4"/>
-      <c r="B1" s="120"/>
-      <c r="C1" s="121"/>
-      <c r="D1" s="122" t="s">
+      <c r="B1" s="128"/>
+      <c r="C1" s="129"/>
+      <c r="D1" s="130" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="122"/>
-      <c r="F1" s="122"/>
-      <c r="G1" s="122"/>
+      <c r="E1" s="130"/>
+      <c r="F1" s="130"/>
+      <c r="G1" s="130"/>
     </row>
     <row r="2" spans="1:9" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -1783,31 +1842,33 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="123" t="s">
+      <c r="A3" s="131" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="123"/>
-      <c r="C3" s="123"/>
-      <c r="D3" s="123"/>
-      <c r="E3" s="123"/>
-      <c r="F3" s="123"/>
-      <c r="G3" s="123"/>
+      <c r="B3" s="131"/>
+      <c r="C3" s="131"/>
+      <c r="D3" s="131"/>
+      <c r="E3" s="131"/>
+      <c r="F3" s="131"/>
+      <c r="G3" s="131"/>
     </row>
     <row r="4" spans="1:9" s="3" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="108" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="109"/>
-      <c r="C4" s="116"/>
-      <c r="D4" s="116"/>
+      <c r="B4" s="109" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="135"/>
+      <c r="D4" s="135"/>
       <c r="E4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="125">
+      <c r="F4" s="133">
         <f ca="1">TODAY()</f>
-        <v>43147</v>
-      </c>
-      <c r="G4" s="125"/>
+        <v>43150</v>
+      </c>
+      <c r="G4" s="133"/>
     </row>
     <row r="5" spans="1:9" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="83" t="s">
@@ -1819,10 +1880,10 @@
       <c r="E5" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="115" t="s">
+      <c r="F5" s="134" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="115"/>
+      <c r="G5" s="134"/>
       <c r="H5" s="53"/>
     </row>
     <row r="6" spans="1:9" s="3" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -1835,18 +1896,18 @@
       <c r="E6" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="115" t="s">
+      <c r="F6" s="134" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="115"/>
+      <c r="G6" s="134"/>
       <c r="I6" s="53"/>
     </row>
     <row r="7" spans="1:9" s="3" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="124"/>
-      <c r="C7" s="124"/>
+      <c r="B7" s="132"/>
+      <c r="C7" s="132"/>
       <c r="D7" s="87"/>
       <c r="E7" s="28" t="s">
         <v>9</v>
@@ -1862,17 +1923,17 @@
       <c r="E8" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="119"/>
-      <c r="G8" s="119"/>
+      <c r="F8" s="138"/>
+      <c r="G8" s="138"/>
     </row>
     <row r="9" spans="1:9" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="88" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="118" t="s">
+      <c r="B9" s="137" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="118"/>
+      <c r="C9" s="137"/>
       <c r="D9" s="89"/>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
@@ -1925,11 +1986,11 @@
       <c r="A14" s="111" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="117" t="s">
+      <c r="B14" s="136" t="s">
         <v>69</v>
       </c>
-      <c r="C14" s="117"/>
-      <c r="D14" s="117"/>
+      <c r="C14" s="136"/>
+      <c r="D14" s="136"/>
       <c r="E14" s="112" t="s">
         <v>3</v>
       </c>
@@ -1941,27 +2002,45 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="98"/>
-      <c r="B15" s="114"/>
-      <c r="C15" s="114"/>
-      <c r="D15" s="114"/>
-      <c r="E15" s="100"/>
-      <c r="F15" s="100"/>
+      <c r="A15" s="98">
+        <v>43150</v>
+      </c>
+      <c r="B15" s="148" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="149"/>
+      <c r="D15" s="147" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" s="150">
+        <v>2</v>
+      </c>
+      <c r="F15" s="100">
+        <v>18.95</v>
+      </c>
       <c r="G15" s="100">
         <f>E15*F15</f>
-        <v>0</v>
+        <v>37.9</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="101"/>
-      <c r="B16" s="102"/>
-      <c r="C16" s="102"/>
-      <c r="D16" s="102"/>
-      <c r="E16" s="103"/>
-      <c r="F16" s="104"/>
+      <c r="B16" s="151" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="152"/>
+      <c r="D16" s="153" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" s="103">
+        <v>4</v>
+      </c>
+      <c r="F16" s="104">
+        <v>4.99</v>
+      </c>
       <c r="G16" s="105">
         <f>E16*F16</f>
-        <v>0</v>
+        <v>19.96</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -2123,57 +2202,57 @@
       <c r="F30" s="43"/>
       <c r="G30" s="57">
         <f>SUM(G15:G28)</f>
-        <v>0</v>
+        <v>57.86</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="130" t="s">
+      <c r="A31" s="118" t="s">
         <v>17</v>
       </c>
-      <c r="B31" s="130"/>
-      <c r="C31" s="130"/>
+      <c r="B31" s="118"/>
+      <c r="C31" s="118"/>
       <c r="D31" s="12"/>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
       <c r="G31" s="44"/>
     </row>
     <row r="32" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="133" t="s">
+      <c r="A32" s="121" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="134"/>
-      <c r="C32" s="134"/>
-      <c r="D32" s="134"/>
-      <c r="E32" s="134"/>
-      <c r="F32" s="134"/>
-      <c r="G32" s="135"/>
+      <c r="B32" s="122"/>
+      <c r="C32" s="122"/>
+      <c r="D32" s="122"/>
+      <c r="E32" s="122"/>
+      <c r="F32" s="122"/>
+      <c r="G32" s="123"/>
     </row>
     <row r="33" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="136"/>
-      <c r="B33" s="136"/>
-      <c r="C33" s="136"/>
-      <c r="D33" s="136"/>
-      <c r="E33" s="136"/>
-      <c r="F33" s="136"/>
-      <c r="G33" s="137"/>
+      <c r="A33" s="124"/>
+      <c r="B33" s="124"/>
+      <c r="C33" s="124"/>
+      <c r="D33" s="124"/>
+      <c r="E33" s="124"/>
+      <c r="F33" s="124"/>
+      <c r="G33" s="125"/>
     </row>
     <row r="34" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="136"/>
-      <c r="B34" s="136"/>
-      <c r="C34" s="136"/>
-      <c r="D34" s="136"/>
-      <c r="E34" s="136"/>
-      <c r="F34" s="136"/>
-      <c r="G34" s="137"/>
+      <c r="A34" s="124"/>
+      <c r="B34" s="124"/>
+      <c r="C34" s="124"/>
+      <c r="D34" s="124"/>
+      <c r="E34" s="124"/>
+      <c r="F34" s="124"/>
+      <c r="G34" s="125"/>
     </row>
     <row r="35" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="138"/>
-      <c r="B35" s="138"/>
-      <c r="C35" s="138"/>
-      <c r="D35" s="138"/>
-      <c r="E35" s="138"/>
-      <c r="F35" s="138"/>
-      <c r="G35" s="139"/>
+      <c r="A35" s="126"/>
+      <c r="B35" s="126"/>
+      <c r="C35" s="126"/>
+      <c r="D35" s="126"/>
+      <c r="E35" s="126"/>
+      <c r="F35" s="126"/>
+      <c r="G35" s="127"/>
     </row>
     <row r="36" spans="1:10" ht="6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="41"/>
@@ -2230,14 +2309,14 @@
       <c r="A41" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B41" s="126"/>
-      <c r="C41" s="132"/>
-      <c r="D41" s="127"/>
+      <c r="B41" s="114"/>
+      <c r="C41" s="120"/>
+      <c r="D41" s="115"/>
       <c r="E41" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="F41" s="126"/>
-      <c r="G41" s="127"/>
+      <c r="F41" s="114"/>
+      <c r="G41" s="115"/>
       <c r="J41" s="21" t="s">
         <v>16</v>
       </c>
@@ -2252,10 +2331,10 @@
       <c r="G42" s="25"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="131" t="s">
+      <c r="A43" s="119" t="s">
         <v>18</v>
       </c>
-      <c r="B43" s="131"/>
+      <c r="B43" s="119"/>
       <c r="C43" s="50"/>
       <c r="D43" s="51"/>
       <c r="E43" s="52"/>
@@ -2297,13 +2376,13 @@
       <c r="A47" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="B47" s="128"/>
-      <c r="C47" s="129"/>
+      <c r="B47" s="116"/>
+      <c r="C47" s="117"/>
       <c r="D47" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E47" s="128"/>
-      <c r="F47" s="129"/>
+      <c r="E47" s="116"/>
+      <c r="F47" s="117"/>
       <c r="G47" s="33"/>
     </row>
     <row r="48" spans="1:10" s="5" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2340,7 +2419,20 @@
     <row r="53" spans="1:7" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
     <row r="54" spans="1:7" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="20">
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="C4:D4"/>
     <mergeCell ref="F41:G41"/>
     <mergeCell ref="E47:F47"/>
     <mergeCell ref="B47:C47"/>
@@ -2348,35 +2440,26 @@
     <mergeCell ref="A43:B43"/>
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="A32:G35"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="F8:G8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A39" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D15" r:id="rId2" xr:uid="{CA7AEC52-BFE5-4C20-A8A4-A628806486A0}"/>
+    <hyperlink ref="D16" r:id="rId3" xr:uid="{88C39F67-ECC8-4908-AA1A-D2A62B3A0F25}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.3" footer="0.3"/>
-  <pageSetup scale="95" orientation="portrait" r:id="rId2"/>
+  <pageSetup scale="95" orientation="portrait" r:id="rId4"/>
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;RRevised 7/31/14</oddFooter>
   </headerFooter>
-  <drawing r:id="rId3"/>
-  <legacyDrawing r:id="rId4"/>
+  <drawing r:id="rId5"/>
+  <legacyDrawing r:id="rId6"/>
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId5" name="CheckBox1">
-          <controlPr autoLine="0" autoPict="0" r:id="rId6">
+        <control shapeId="1025" r:id="rId7" name="CheckBox1">
+          <controlPr autoLine="0" autoPict="0" r:id="rId8">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -2395,7 +2478,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId5" name="CheckBox1"/>
+        <control shapeId="1025" r:id="rId7" name="CheckBox1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -2447,7 +2530,7 @@
       <c r="A3" s="63">
         <v>1</v>
       </c>
-      <c r="B3" s="140" t="s">
+      <c r="B3" s="139" t="s">
         <v>34</v>
       </c>
       <c r="C3" s="59" t="s">
@@ -2458,7 +2541,7 @@
       <c r="A4" s="63">
         <v>2</v>
       </c>
-      <c r="B4" s="140"/>
+      <c r="B4" s="139"/>
       <c r="C4" s="72" t="s">
         <v>47</v>
       </c>
@@ -2467,7 +2550,7 @@
       <c r="A5" s="63">
         <v>3</v>
       </c>
-      <c r="B5" s="141"/>
+      <c r="B5" s="140"/>
       <c r="C5" s="59" t="s">
         <v>50</v>
       </c>
@@ -2476,7 +2559,7 @@
       <c r="A6" s="63">
         <v>4</v>
       </c>
-      <c r="B6" s="141"/>
+      <c r="B6" s="140"/>
       <c r="C6" s="59" t="s">
         <v>54</v>
       </c>
@@ -2485,7 +2568,7 @@
       <c r="A7" s="63">
         <v>5</v>
       </c>
-      <c r="B7" s="141"/>
+      <c r="B7" s="140"/>
       <c r="C7" s="67" t="s">
         <v>55</v>
       </c>
@@ -2494,11 +2577,11 @@
       <c r="A8" s="68">
         <v>6</v>
       </c>
-      <c r="B8" s="141"/>
+      <c r="B8" s="140"/>
       <c r="C8" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="144"/>
+      <c r="E8" s="143"/>
     </row>
     <row r="9" spans="1:5" s="75" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="68">
@@ -2508,18 +2591,18 @@
       <c r="C9" s="73" t="s">
         <v>58</v>
       </c>
-      <c r="E9" s="144"/>
+      <c r="E9" s="143"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="63"/>
       <c r="B10" s="63"/>
-      <c r="E10" s="145"/>
+      <c r="E10" s="144"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="63">
         <v>7</v>
       </c>
-      <c r="B11" s="140" t="s">
+      <c r="B11" s="139" t="s">
         <v>35</v>
       </c>
       <c r="C11" s="59" t="s">
@@ -2528,13 +2611,13 @@
       <c r="D11" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="145"/>
+      <c r="E11" s="144"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="63">
         <v>7.1</v>
       </c>
-      <c r="B12" s="141"/>
+      <c r="B12" s="140"/>
       <c r="C12" s="69" t="s">
         <v>30</v>
       </c>
@@ -2543,50 +2626,50 @@
       <c r="A13" s="63">
         <v>8</v>
       </c>
-      <c r="B13" s="141"/>
+      <c r="B13" s="140"/>
       <c r="C13" s="59" t="s">
         <v>43</v>
       </c>
       <c r="D13" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="146"/>
+      <c r="E13" s="145"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="63">
         <v>8.1</v>
       </c>
-      <c r="B14" s="141"/>
+      <c r="B14" s="140"/>
       <c r="C14" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="147"/>
+      <c r="E14" s="146"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="63">
         <v>9</v>
       </c>
-      <c r="B15" s="141"/>
+      <c r="B15" s="140"/>
       <c r="C15" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="147"/>
+      <c r="E15" s="146"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="63">
         <v>10</v>
       </c>
-      <c r="B16" s="141"/>
+      <c r="B16" s="140"/>
       <c r="C16" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="147"/>
+      <c r="E16" s="146"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="63">
         <v>11</v>
       </c>
-      <c r="B17" s="141"/>
+      <c r="B17" s="140"/>
       <c r="C17" s="59" t="s">
         <v>49</v>
       </c>
@@ -2596,7 +2679,7 @@
       <c r="A18" s="68">
         <v>12</v>
       </c>
-      <c r="B18" s="141"/>
+      <c r="B18" s="140"/>
       <c r="C18" s="75" t="s">
         <v>53</v>
       </c>
@@ -2605,7 +2688,7 @@
       <c r="A19" s="68">
         <v>13</v>
       </c>
-      <c r="B19" s="141"/>
+      <c r="B19" s="140"/>
       <c r="C19" s="75" t="s">
         <v>52</v>
       </c>
@@ -2614,7 +2697,7 @@
       <c r="A20" s="63">
         <v>14</v>
       </c>
-      <c r="B20" s="141"/>
+      <c r="B20" s="140"/>
       <c r="C20" s="59" t="s">
         <v>45</v>
       </c>
@@ -2623,7 +2706,7 @@
       <c r="A21" s="63">
         <v>15</v>
       </c>
-      <c r="B21" s="141"/>
+      <c r="B21" s="140"/>
       <c r="C21" s="59" t="s">
         <v>38</v>
       </c>
@@ -2632,7 +2715,7 @@
       <c r="A22" s="63">
         <v>16</v>
       </c>
-      <c r="B22" s="141"/>
+      <c r="B22" s="140"/>
       <c r="C22" s="59" t="s">
         <v>44</v>
       </c>
@@ -2645,7 +2728,7 @@
       <c r="A24" s="63">
         <v>17</v>
       </c>
-      <c r="B24" s="142" t="s">
+      <c r="B24" s="141" t="s">
         <v>36</v>
       </c>
       <c r="C24" s="59" t="s">
@@ -2656,7 +2739,7 @@
       <c r="A25" s="63">
         <v>18</v>
       </c>
-      <c r="B25" s="143"/>
+      <c r="B25" s="142"/>
       <c r="C25" s="59" t="s">
         <v>33</v>
       </c>
@@ -2665,7 +2748,7 @@
       <c r="A26" s="63">
         <v>19</v>
       </c>
-      <c r="B26" s="143"/>
+      <c r="B26" s="142"/>
       <c r="C26" s="59" t="s">
         <v>39</v>
       </c>
@@ -2678,7 +2761,7 @@
       <c r="A28" s="63">
         <v>20</v>
       </c>
-      <c r="B28" s="140" t="s">
+      <c r="B28" s="139" t="s">
         <v>37</v>
       </c>
       <c r="C28" s="59" t="s">
@@ -2689,14 +2772,14 @@
       <c r="A29" s="63">
         <v>21</v>
       </c>
-      <c r="B29" s="141"/>
+      <c r="B29" s="140"/>
       <c r="C29" s="59" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="63"/>
-      <c r="B30" s="141"/>
+      <c r="B30" s="140"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="63"/>

</xml_diff>